<commit_message>
[Phatnttse][Update Export To Excel]
</commit_message>
<xml_diff>
--- a/Bonheur.API/Templates/SupplierListTemplate.xlsx
+++ b/Bonheur.API/Templates/SupplierListTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,82 +57,82 @@
     <t>[[%Field:Priority%]]</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Slug</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>Province</t>
-  </si>
-  <si>
-    <t>Ward</t>
-  </si>
-  <si>
-    <t>District</t>
-  </si>
-  <si>
     <t>Website</t>
   </si>
   <si>
-    <t>Response Time</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>IsFeatured</t>
-  </si>
-  <si>
     <t>[[%Field:IsFeatured%]]</t>
   </si>
   <si>
-    <t>ProrityEnd</t>
-  </si>
-  <si>
     <t>[[%Field:ProrityEnd%]]</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>[[%Field:Status%]]</t>
   </si>
   <si>
-    <t>OnBoardStatus</t>
-  </si>
-  <si>
     <t>[[%Field:OnBoardStatus%]]</t>
   </si>
   <si>
-    <t>Discount</t>
-  </si>
-  <si>
     <t>[[%Field:Discount%]]</t>
   </si>
   <si>
-    <t>AverageRating</t>
-  </si>
-  <si>
     <t>[[%Field:AverageRating%]]</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>[[%Field:Category.Name%]]</t>
+  </si>
+  <si>
+    <t>Danh mục</t>
+  </si>
+  <si>
+    <t>Tên nhà cung cấp</t>
+  </si>
+  <si>
+    <t>Đường dẫn</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Giá</t>
+  </si>
+  <si>
+    <t>Địa chỉ chi tiết</t>
+  </si>
+  <si>
+    <t>Tỉnh/Thành phố</t>
+  </si>
+  <si>
+    <t>Quận/Huyện</t>
+  </si>
+  <si>
+    <t>Phường/Xã</t>
+  </si>
+  <si>
+    <t>Thời gian phản hồi</t>
+  </si>
+  <si>
+    <t>Chỉ số ưu tiên</t>
+  </si>
+  <si>
+    <t>Nổi bật</t>
+  </si>
+  <si>
+    <t>Thời gian kết thúc ưu tiên</t>
+  </si>
+  <si>
+    <t>Trạng thái duyệt</t>
+  </si>
+  <si>
+    <t>Trạng thái hoàn thành</t>
+  </si>
+  <si>
+    <t>Giảm giá</t>
+  </si>
+  <si>
+    <t>Đánh giá</t>
   </si>
 </sst>
 </file>
@@ -477,92 +477,94 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>37</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -586,10 +588,10 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
         <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
       </c>
       <c r="K2" t="s">
         <v>9</v>
@@ -601,22 +603,22 @@
         <v>11</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="O2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="P2" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="S2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>